<commit_message>
tweak legend tab name, hyperlink logo
</commit_message>
<xml_diff>
--- a/src/downloads/SPAR data, 2010-2017 - 052020.xlsx
+++ b/src/downloads/SPAR data, 2010-2017 - 052020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikevanmaele/Documents/GitHub/gida-landing/src/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBDE291B-71E6-7E4D-8F0A-79EC3A51BD63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2812A316-5804-5F46-844C-0629B7B838F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4747" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4747" uniqueCount="450">
   <si>
     <t>Country</t>
   </si>
@@ -1447,6 +1447,9 @@
   <si>
     <t>Last updated 2020-05-20</t>
   </si>
+  <si>
+    <t>Legend for SPAR data</t>
+  </si>
 </sst>
 </file>
 
@@ -1780,6 +1783,9 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1799,9 +1805,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1846,6 +1849,7 @@
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A9591EC-52CD-5E48-9B4F-0546E22BCA47}"/>
@@ -1857,7 +1861,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:clrChange>
             <a:clrFrom>
               <a:srgbClr val="FFFFFF"/>
@@ -2202,9 +2206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272FF391-350C-7040-AA4E-ABC7B5554BAA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
@@ -2239,7 +2241,7 @@
     <row r="5" spans="1:4" s="11" customFormat="1" ht="272" customHeight="1" thickBot="1">
       <c r="A5"/>
       <c r="B5" s="18"/>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="24" t="s">
         <v>447</v>
       </c>
       <c r="D5" s="19"/>
@@ -2288,41 +2290,41 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="70" customHeight="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>401</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:17" ht="15" thickBot="1"/>
     <row r="6" spans="1:17" ht="38" customHeight="1" thickBot="1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>399</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="24" t="s">
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="25" t="s">
         <v>441</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27" t="s">
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28" t="s">
         <v>442</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="24" t="s">
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="25" t="s">
         <v>443</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="27" t="s">
+      <c r="M6" s="26"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="28" t="s">
         <v>440</v>
       </c>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30"/>
     </row>
     <row r="7" spans="1:17" ht="40" customHeight="1" thickBot="1">
       <c r="A7" s="6" t="s">
@@ -84670,7 +84672,7 @@
     <row r="1" spans="1:18" ht="90" customHeight="1"/>
     <row r="2" spans="1:18" ht="34">
       <c r="A2" s="2" t="s">
-        <v>400</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="24">
@@ -84679,41 +84681,41 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="70" customHeight="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>405</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:18" ht="15" thickBot="1"/>
     <row r="6" spans="1:18" ht="38" customHeight="1" thickBot="1">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>399</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="24" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="25" t="s">
         <v>441</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27" t="s">
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="28" t="s">
         <v>442</v>
       </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="24" t="s">
+      <c r="K6" s="29"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="25" t="s">
         <v>443</v>
       </c>
-      <c r="N6" s="25"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="27" t="s">
+      <c r="N6" s="26"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="28" t="s">
         <v>440</v>
       </c>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="30"/>
     </row>
     <row r="7" spans="1:18" ht="40" customHeight="1" thickBot="1">
       <c r="A7" s="6" t="s">

</xml_diff>